<commit_message>
Update Set Points in USE_TYPE_PROPERTIES for all UD scenarios
</commit_message>
<xml_diff>
--- a/remap_ville_plugin/CH_ReMaP/archetypes/URB_2040_BAU/use_types/USE_TYPE_PROPERTIES.xlsx
+++ b/remap_ville_plugin/CH_ReMaP/archetypes/URB_2040_BAU/use_types/USE_TYPE_PROPERTIES.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shsieh\Documents\GitHub\cea-remap-ville-plugin\remap_ville_plugin\CH_ReMaP\archetypes\URB_2040_BAU\use_types\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aoraiopoulos\Documents\GitHub\cea-remap-ville-plugin\remap_ville_plugin\CH_ReMaP\archetypes\URB_2040_BAU\use_types\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6A2B79-51A1-4855-9D1C-0E66740B7BCC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98A44313-2E6E-44D5-91E9-EEC58A9F45D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21420" yWindow="1035" windowWidth="17280" windowHeight="13980" tabRatio="785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INTERNAL_LOADS" sheetId="1" r:id="rId1"/>
@@ -551,29 +551,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.453125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7265625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="1" customWidth="1"/>
     <col min="6" max="6" width="10" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.1796875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7265625" style="1" customWidth="1"/>
-    <col min="12" max="13" width="12.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.1796875" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.1796875" style="1"/>
+    <col min="7" max="7" width="11.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" style="1" customWidth="1"/>
+    <col min="12" max="13" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -617,7 +617,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>14</v>
       </c>
@@ -661,7 +661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>40</v>
       </c>
@@ -705,7 +705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>15</v>
       </c>
@@ -749,7 +749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>16</v>
       </c>
@@ -793,7 +793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>17</v>
       </c>
@@ -837,7 +837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>18</v>
       </c>
@@ -882,7 +882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>19</v>
       </c>
@@ -927,7 +927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>20</v>
       </c>
@@ -971,7 +971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>21</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>22</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>23</v>
       </c>
@@ -1108,7 +1108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>24</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>25</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>26</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>27</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>28</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>29</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>30</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>31</v>
       </c>
@@ -1463,7 +1463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>32</v>
       </c>
@@ -1517,25 +1517,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.1796875" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.1796875" style="1"/>
+    <col min="6" max="6" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1561,15 +1561,15 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C2" s="4">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2" s="2">
         <v>28</v>
@@ -1588,15 +1588,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>40</v>
       </c>
       <c r="B3" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C3" s="4">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" s="2">
         <v>28</v>
@@ -1615,15 +1615,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C4" s="4">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" s="2">
         <v>28</v>
@@ -1642,15 +1642,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C5" s="4">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="2">
         <v>28</v>
@@ -1669,15 +1669,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C6" s="4">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" s="2">
         <v>28</v>
@@ -1696,15 +1696,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C7" s="4">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" s="2">
         <v>28</v>
@@ -1723,15 +1723,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C8" s="4">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" s="2">
         <v>28</v>
@@ -1750,15 +1750,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C9" s="4">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" s="2">
         <v>28</v>
@@ -1777,15 +1777,15 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="2">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C10" s="4">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" s="2">
         <v>32</v>
@@ -1804,15 +1804,15 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C11" s="4">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" s="2">
         <v>28</v>
@@ -1831,7 +1831,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>23</v>
       </c>
@@ -1858,15 +1858,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B13" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C13" s="4">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" s="2">
         <v>28</v>
@@ -1885,15 +1885,15 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B14" s="2">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C14" s="4">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D14" s="2">
         <v>32</v>
@@ -1912,15 +1912,15 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B15" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C15" s="4">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D15" s="2">
         <v>28</v>
@@ -1938,15 +1938,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B16" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C16" s="4">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D16" s="2">
         <v>28</v>
@@ -1964,7 +1964,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>28</v>
       </c>
@@ -1990,15 +1990,15 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B18" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C18" s="4">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D18" s="2">
         <v>28</v>
@@ -2017,15 +2017,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B19" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C19" s="4">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D19" s="2">
         <v>28</v>
@@ -2044,15 +2044,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B20" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C20" s="4">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D20" s="2">
         <v>28</v>
@@ -2071,15 +2071,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B21" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C21" s="4">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D21" s="2">
         <v>28</v>

</xml_diff>